<commit_message>
updated with done functionalities
</commit_message>
<xml_diff>
--- a/DOCS/Use Cases/Estimation.xlsx
+++ b/DOCS/Use Cases/Estimation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>UC</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Restore from backup</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -538,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,7 +553,7 @@
     <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,7 +573,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -585,8 +588,11 @@
         <f>E2/E40</f>
         <v>3.7037037037037035E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -601,8 +607,11 @@
         <f>E3/E40</f>
         <v>3.7037037037037035E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -618,7 +627,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -634,7 +643,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -650,7 +659,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -666,7 +675,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -682,7 +691,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -698,7 +707,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -713,8 +722,11 @@
         <f>E10/E40</f>
         <v>1.8518518518518517E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -730,7 +742,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -745,8 +757,11 @@
         <f>E12/E40</f>
         <v>1.8518518518518517E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -761,8 +776,11 @@
         <f>E13/E40</f>
         <v>1.8518518518518517E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -777,8 +795,11 @@
         <f>E14/E40</f>
         <v>1.8518518518518517E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -794,7 +815,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -810,7 +831,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -826,7 +847,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -842,7 +863,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -858,7 +879,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -874,7 +895,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -890,7 +911,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -906,7 +927,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -921,8 +942,11 @@
         <f>E23/E40</f>
         <v>1.8518518518518517E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -938,7 +962,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -954,7 +978,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -970,7 +994,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -986,7 +1010,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1002,7 +1026,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1017,8 +1041,11 @@
         <f>E29/E40</f>
         <v>1.8518518518518517E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1034,7 +1061,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1050,7 +1077,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>44</v>
       </c>

</xml_diff>